<commit_message>
Added controls w/ plots
</commit_message>
<xml_diff>
--- a/data/ap_data.xlsx
+++ b/data/ap_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t xml:space="preserve">ml_amount</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">ap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">control</t>
   </si>
 </sst>
 </file>
@@ -112,7 +115,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,7 +143,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -161,7 +164,9 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -173,6 +178,9 @@
       <c r="C2" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -184,6 +192,9 @@
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -195,6 +206,9 @@
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -206,6 +220,9 @@
       <c r="C5" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -217,6 +234,9 @@
       <c r="C6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -228,6 +248,9 @@
       <c r="C7" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -239,6 +262,9 @@
       <c r="C8" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -250,6 +276,9 @@
       <c r="C9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -261,6 +290,9 @@
       <c r="C10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -272,6 +304,9 @@
       <c r="C11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -283,6 +318,9 @@
       <c r="C12" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -294,6 +332,9 @@
       <c r="C13" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -305,6 +346,9 @@
       <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -316,6 +360,9 @@
       <c r="C15" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -325,6 +372,9 @@
         <v>2.5</v>
       </c>
       <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -338,6 +388,9 @@
       <c r="C17" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -349,7 +402,9 @@
       <c r="C18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,6 +417,9 @@
       <c r="C19" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -373,6 +431,9 @@
       <c r="C20" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -384,6 +445,9 @@
       <c r="C21" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -395,6 +459,9 @@
       <c r="C22" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -406,6 +473,9 @@
       <c r="C23" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -417,6 +487,9 @@
       <c r="C24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -428,6 +501,9 @@
       <c r="C25" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D25" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -439,6 +515,9 @@
       <c r="C26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -450,6 +529,9 @@
       <c r="C27" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D27" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -461,6 +543,9 @@
       <c r="C28" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -472,6 +557,9 @@
       <c r="C29" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D29" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -483,6 +571,9 @@
       <c r="C30" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -494,6 +585,9 @@
       <c r="C31" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D31" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -505,6 +599,9 @@
       <c r="C32" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -516,6 +613,9 @@
       <c r="C33" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -525,6 +625,9 @@
         <v>2.5</v>
       </c>
       <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -544,13 +647,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -562,6 +665,9 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -573,6 +679,9 @@
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -584,6 +693,9 @@
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -595,6 +707,9 @@
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -606,6 +721,9 @@
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -617,6 +735,9 @@
       <c r="C6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -628,6 +749,9 @@
       <c r="C7" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -639,6 +763,9 @@
       <c r="C8" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -650,6 +777,9 @@
       <c r="C9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -661,6 +791,9 @@
       <c r="C10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -672,6 +805,9 @@
       <c r="C11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -683,6 +819,9 @@
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -694,6 +833,9 @@
       <c r="C13" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -705,6 +847,9 @@
       <c r="C14" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -716,6 +861,9 @@
       <c r="C15" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -726,6 +874,9 @@
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,6 +889,9 @@
       <c r="C17" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -749,6 +903,9 @@
       <c r="C18" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -760,6 +917,9 @@
       <c r="C19" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -771,6 +931,9 @@
       <c r="C20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -782,6 +945,9 @@
       <c r="C21" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -793,6 +959,9 @@
       <c r="C22" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -804,6 +973,9 @@
       <c r="C23" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -815,6 +987,9 @@
       <c r="C24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -826,6 +1001,9 @@
       <c r="C25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D25" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -837,6 +1015,9 @@
       <c r="C26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D26" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -848,6 +1029,9 @@
       <c r="C27" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D27" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -859,6 +1043,9 @@
       <c r="C28" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D28" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -870,6 +1057,9 @@
       <c r="C29" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D29" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -881,6 +1071,9 @@
       <c r="C30" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D30" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -892,6 +1085,9 @@
       <c r="C31" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D31" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -903,6 +1099,9 @@
       <c r="C32" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D32" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -914,6 +1113,9 @@
       <c r="C33" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D33" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -924,6 +1126,9 @@
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -946,13 +1151,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -964,6 +1169,9 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -975,6 +1183,9 @@
       <c r="C2" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -986,6 +1197,9 @@
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -997,6 +1211,9 @@
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1008,6 +1225,9 @@
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1019,6 +1239,9 @@
       <c r="C6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1030,6 +1253,9 @@
       <c r="C7" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1041,6 +1267,9 @@
       <c r="C8" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1052,6 +1281,9 @@
       <c r="C9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1063,6 +1295,9 @@
       <c r="C10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -1074,6 +1309,9 @@
       <c r="C11" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -1085,6 +1323,9 @@
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -1096,6 +1337,9 @@
       <c r="C13" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1107,6 +1351,9 @@
       <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1118,6 +1365,9 @@
       <c r="C15" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -1128,6 +1378,9 @@
       </c>
       <c r="C16" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1140,6 +1393,9 @@
       <c r="C17" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -1151,6 +1407,9 @@
       <c r="C18" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -1162,6 +1421,9 @@
       <c r="C19" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1173,6 +1435,9 @@
       <c r="C20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -1184,6 +1449,9 @@
       <c r="C21" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -1195,6 +1463,9 @@
       <c r="C22" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -1206,6 +1477,9 @@
       <c r="C23" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -1217,6 +1491,9 @@
       <c r="C24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -1228,6 +1505,9 @@
       <c r="C25" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D25" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -1239,6 +1519,9 @@
       <c r="C26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -1250,6 +1533,9 @@
       <c r="C27" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D27" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -1261,6 +1547,9 @@
       <c r="C28" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D28" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -1272,6 +1561,9 @@
       <c r="C29" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D29" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -1283,6 +1575,9 @@
       <c r="C30" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D30" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -1294,6 +1589,9 @@
       <c r="C31" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D31" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -1305,6 +1603,9 @@
       <c r="C32" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D32" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -1316,6 +1617,9 @@
       <c r="C33" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D33" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -1326,6 +1630,9 @@
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1348,13 +1655,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1366,6 +1673,9 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -1377,6 +1687,9 @@
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -1388,6 +1701,9 @@
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1399,6 +1715,9 @@
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1410,6 +1729,9 @@
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1421,6 +1743,9 @@
       <c r="C6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1432,6 +1757,9 @@
       <c r="C7" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D7" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1443,6 +1771,9 @@
       <c r="C8" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1454,6 +1785,9 @@
       <c r="C9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1465,6 +1799,9 @@
       <c r="C10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D10" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -1476,6 +1813,9 @@
       <c r="C11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -1487,6 +1827,9 @@
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -1498,6 +1841,9 @@
       <c r="C13" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D13" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1509,6 +1855,9 @@
       <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1520,6 +1869,9 @@
       <c r="C15" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -1530,6 +1882,9 @@
       </c>
       <c r="C16" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,6 +1897,9 @@
       <c r="C17" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -1553,6 +1911,9 @@
       <c r="C18" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -1564,6 +1925,9 @@
       <c r="C19" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1575,6 +1939,9 @@
       <c r="C20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -1586,6 +1953,9 @@
       <c r="C21" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -1597,6 +1967,9 @@
       <c r="C22" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D22" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -1608,6 +1981,9 @@
       <c r="C23" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D23" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -1619,6 +1995,9 @@
       <c r="C24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D24" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -1630,6 +2009,9 @@
       <c r="C25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D25" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -1641,6 +2023,9 @@
       <c r="C26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -1652,6 +2037,9 @@
       <c r="C27" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D27" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -1663,6 +2051,9 @@
       <c r="C28" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D28" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -1674,6 +2065,9 @@
       <c r="C29" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D29" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -1685,6 +2079,9 @@
       <c r="C30" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D30" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -1696,6 +2093,9 @@
       <c r="C31" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D31" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -1707,6 +2107,9 @@
       <c r="C32" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D32" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -1718,6 +2121,9 @@
       <c r="C33" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D33" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -1728,6 +2134,9 @@
       </c>
       <c r="C34" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>